<commit_message>
some fixes in evaluation form
</commit_message>
<xml_diff>
--- a/evaluation/go-no/evaluation.xlsx
+++ b/evaluation/go-no/evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0ca65449af92ce79/!FH/MA/git/WakeWordPicoW/evaluation/go-no/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="8_{F9D07428-2867-48BC-B9E2-8CCBF4F4083D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96F34F41-1FA7-42CA-9915-D12DE23F6740}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="8_{F9D07428-2867-48BC-B9E2-8CCBF4F4083D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67EEDAF9-947B-40AC-98F3-F2AEDBB34EA6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFF0A4DB-B991-4289-9116-52795F214A99}"/>
+    <workbookView xWindow="-15060" yWindow="60" windowWidth="12150" windowHeight="15600" xr2:uid="{FFF0A4DB-B991-4289-9116-52795F214A99}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="6">
   <si>
     <t>go</t>
   </si>
@@ -47,9 +47,6 @@
     <t>wrong</t>
   </si>
   <si>
-    <t>nothing</t>
-  </si>
-  <si>
     <t>word</t>
   </si>
   <si>
@@ -57,12 +54,6 @@
   </si>
   <si>
     <t>no</t>
-  </si>
-  <si>
-    <t>free</t>
-  </si>
-  <si>
-    <t>total</t>
   </si>
 </sst>
 </file>
@@ -115,6 +106,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -434,36 +429,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE5381C8-FE10-4903-8C08-1A4C39DC53A3}">
-  <dimension ref="B1:E45"/>
+  <dimension ref="B3:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1">
-        <v>2.4400000000000002E-2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C2">
-        <v>168782</v>
-      </c>
-      <c r="D2">
-        <v>34456</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -471,145 +447,142 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -617,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -625,10 +598,10 @@
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -636,7 +609,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -644,10 +617,10 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -655,10 +628,10 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -666,10 +639,10 @@
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -677,10 +650,10 @@
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -688,214 +661,214 @@
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the colums of evaluation
for a better overview
</commit_message>
<xml_diff>
--- a/evaluation/go-no/evaluation.xlsx
+++ b/evaluation/go-no/evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0ca65449af92ce79/!FH/MA/git/WakeWordPicoW/evaluation/go-no/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="8_{F9D07428-2867-48BC-B9E2-8CCBF4F4083D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67EEDAF9-947B-40AC-98F3-F2AEDBB34EA6}"/>
+  <xr:revisionPtr revIDLastSave="193" documentId="8_{F9D07428-2867-48BC-B9E2-8CCBF4F4083D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA82F2C5-D59E-4DBF-9554-D1017994DD6D}"/>
   <bookViews>
-    <workbookView xWindow="-15060" yWindow="60" windowWidth="12150" windowHeight="15600" xr2:uid="{FFF0A4DB-B991-4289-9116-52795F214A99}"/>
+    <workbookView xWindow="5850" yWindow="1275" windowWidth="12150" windowHeight="15600" xr2:uid="{FFF0A4DB-B991-4289-9116-52795F214A99}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="7">
   <si>
     <t>go</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>unclear</t>
   </si>
 </sst>
 </file>
@@ -429,15 +432,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE5381C8-FE10-4903-8C08-1A4C39DC53A3}">
-  <dimension ref="B3:D45"/>
+  <dimension ref="B3:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -447,52 +450,43 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>0</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -500,7 +494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -508,84 +502,63 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>0</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>0</v>
       </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>0</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>0</v>
       </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>0</v>
       </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>0</v>
       </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>0</v>
       </c>
@@ -593,18 +566,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>0</v>
       </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>0</v>
       </c>
@@ -612,73 +582,55 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>0</v>
       </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>0</v>
       </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>0</v>
       </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>0</v>
       </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>0</v>
       </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>5</v>
       </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>5</v>
       </c>
@@ -686,18 +638,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>5</v>
       </c>
-      <c r="C27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>5</v>
       </c>
@@ -705,40 +654,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>5</v>
       </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>5</v>
       </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>5</v>
       </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>5</v>
       </c>
@@ -746,7 +686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>5</v>
       </c>
@@ -754,40 +694,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>5</v>
       </c>
-      <c r="C34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>5</v>
       </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>5</v>
       </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>5</v>
       </c>
@@ -795,51 +726,39 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>5</v>
       </c>
-      <c r="C38" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>5</v>
       </c>
-      <c r="C39" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>5</v>
       </c>
-      <c r="C40" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>5</v>
       </c>
-      <c r="C41" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>5</v>
       </c>
@@ -847,7 +766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>5</v>
       </c>
@@ -855,7 +774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>5</v>
       </c>
@@ -863,7 +782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>5</v>
       </c>

</xml_diff>